<commit_message>
refactor the formate of the xlsx
</commit_message>
<xml_diff>
--- a/src/test/resources/test_error_hearder_file.xlsx
+++ b/src/test/resources/test_error_hearder_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ttzhang/Documents/projects/Natlex_Task/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE305DA-D0F8-5047-B659-571531A7F799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37F8F03-5846-8D44-8184-2CA92B020F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20660" xr2:uid="{C461ED32-CABF-9343-80F3-C9D876E969B0}"/>
   </bookViews>
@@ -486,198 +486,182 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A30A9BAD-409A-184F-A9F9-B12D7A9A0BC3}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.5" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" customWidth="1"/>
-    <col min="4" max="4" width="27.6640625" customWidth="1"/>
-    <col min="5" max="5" width="25.6640625" customWidth="1"/>
-    <col min="6" max="6" width="50.5" customWidth="1"/>
-    <col min="7" max="7" width="23" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="D7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="D9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
+  <mergeCells count="30">
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C7:C8"/>
     <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F5:F6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>